<commit_message>
Added more models and documented results
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="57">
   <si>
     <t>AAPL</t>
   </si>
@@ -145,6 +145,9 @@
     <t>dense_layer</t>
   </si>
   <si>
+    <t>dropout_rate</t>
+  </si>
+  <si>
     <t>loss</t>
   </si>
   <si>
@@ -172,7 +175,16 @@
     <t>mae</t>
   </si>
   <si>
+    <t>adam</t>
+  </si>
+  <si>
+    <t>mse</t>
+  </si>
+  <si>
     <t>adamax</t>
+  </si>
+  <si>
+    <t>rmsprop</t>
   </si>
 </sst>
 </file>
@@ -504,13 +516,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="B1" t="s">
         <v>39</v>
       </c>
@@ -547,198 +559,1683 @@
       <c r="M1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="B2">
+        <v>252</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>224</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>0.9723548611118875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="B3">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>134</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0.2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0.9501156745476711</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="B4">
+        <v>338</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>202</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>0.2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0.9582699610737877</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="B5">
+        <v>160</v>
+      </c>
+      <c r="C5">
+        <v>101</v>
+      </c>
+      <c r="D5">
+        <v>125</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0.1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0.9504124330538782</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="B6">
+        <v>93</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>246</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0.96115939006122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="B7">
+        <v>146</v>
+      </c>
+      <c r="C7">
+        <v>158</v>
+      </c>
+      <c r="D7">
+        <v>150</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>0.2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>0.9081919883983061</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="B8">
+        <v>67</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>86</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>0.2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>0.9267131303970635</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="B9">
+        <v>249</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>200</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>0.4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" t="b">
+        <v>1</v>
+      </c>
+      <c r="M9" t="b">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>0.9672992986824098</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="B10">
+        <v>80</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>235</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>0.3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" t="b">
+        <v>1</v>
+      </c>
+      <c r="M10" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0.971156190647037</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="B11">
+        <v>169</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>114</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>0.1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" t="b">
+        <v>1</v>
+      </c>
+      <c r="M11" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0.8755700150909251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="B12">
+        <v>257</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>123</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>0.5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0.968225173952287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="B13">
+        <v>153</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>132</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>0.4</v>
+      </c>
+      <c r="G13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" t="b">
+        <v>0</v>
+      </c>
+      <c r="M13" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0.8966909817822324</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="B14">
+        <v>205</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>145</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>0.2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>0.9799557670400426</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="B15">
+        <v>52</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>219</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>0.1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" t="b">
+        <v>0</v>
+      </c>
+      <c r="M15" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0.9544293863133937</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <v>110</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>90</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>0.4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" t="b">
+        <v>1</v>
+      </c>
+      <c r="L16" t="b">
+        <v>1</v>
+      </c>
+      <c r="M16" t="b">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>0.8251011798612152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <v>86</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>149</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>0.3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L17" t="b">
+        <v>0</v>
+      </c>
+      <c r="M17" t="b">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0.9822583871954536</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <v>254</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>131</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>0.1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18" t="b">
+        <v>1</v>
+      </c>
+      <c r="M18" t="b">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0.9901075522078303</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19">
+        <v>158</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>241</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>0.1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19" t="b">
+        <v>0</v>
+      </c>
+      <c r="M19" t="b">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>0.9633535767314634</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20">
+        <v>233</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>245</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>0.5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
+      <c r="L20" t="b">
+        <v>0</v>
+      </c>
+      <c r="M20" t="b">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>0.9709357499660785</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21">
+        <v>91</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>108</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0.1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0.9688477999079659</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22">
+        <v>81</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>228</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>0.2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" t="s">
+        <v>53</v>
+      </c>
+      <c r="I22" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="b">
+        <v>0</v>
+      </c>
+      <c r="L22" t="b">
+        <v>0</v>
+      </c>
+      <c r="M22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0.9117900192688089</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23">
+        <v>70</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>135</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>0.1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="b">
+        <v>0</v>
+      </c>
+      <c r="L23" t="b">
+        <v>1</v>
+      </c>
+      <c r="M23" t="b">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0.954180614849984</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24">
+        <v>211</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>73</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>0.5</v>
+      </c>
+      <c r="G24" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24" t="s">
+        <v>53</v>
+      </c>
+      <c r="I24" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="b">
+        <v>0</v>
+      </c>
+      <c r="L24" t="b">
+        <v>1</v>
+      </c>
+      <c r="M24" t="b">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0.9239992251801622</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25">
+        <v>289</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>153</v>
+      </c>
+      <c r="E25">
+        <v>11</v>
+      </c>
+      <c r="F25">
+        <v>0.4</v>
+      </c>
+      <c r="G25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L25" t="b">
+        <v>0</v>
+      </c>
+      <c r="M25" t="b">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0.9751283418089106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26">
+        <v>222</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>75</v>
+      </c>
+      <c r="E26">
+        <v>6</v>
+      </c>
+      <c r="F26">
+        <v>0.5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" t="s">
+        <v>53</v>
+      </c>
+      <c r="I26" t="b">
+        <v>0</v>
+      </c>
+      <c r="J26" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" t="b">
+        <v>0</v>
+      </c>
+      <c r="L26" t="b">
+        <v>0</v>
+      </c>
+      <c r="M26" t="b">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0.9813957773311417</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27">
+        <v>55</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>203</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+      <c r="F27">
+        <v>0.4</v>
+      </c>
+      <c r="G27" t="s">
+        <v>52</v>
+      </c>
+      <c r="H27" t="s">
+        <v>55</v>
+      </c>
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" t="b">
+        <v>1</v>
+      </c>
+      <c r="L27" t="b">
+        <v>1</v>
+      </c>
+      <c r="M27" t="b">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>0.9806609146551855</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28">
+        <v>117</v>
+      </c>
+      <c r="C28">
+        <v>233</v>
+      </c>
+      <c r="D28">
+        <v>212</v>
+      </c>
+      <c r="E28">
+        <v>6</v>
+      </c>
+      <c r="F28">
+        <v>0.1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>52</v>
+      </c>
+      <c r="H28" t="s">
+        <v>53</v>
+      </c>
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" t="b">
+        <v>1</v>
+      </c>
+      <c r="L28" t="b">
+        <v>1</v>
+      </c>
+      <c r="M28" t="b">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>0.9576394501923923</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29">
+        <v>217</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>61</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>0.2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>52</v>
+      </c>
+      <c r="H29" t="s">
+        <v>53</v>
+      </c>
+      <c r="I29" t="b">
+        <v>0</v>
+      </c>
+      <c r="J29" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" t="b">
+        <v>0</v>
+      </c>
+      <c r="L29" t="b">
+        <v>1</v>
+      </c>
+      <c r="M29" t="b">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0.9899385797607924</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30">
+        <v>139</v>
+      </c>
+      <c r="C30">
+        <v>69</v>
+      </c>
+      <c r="D30">
+        <v>111</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="F30">
+        <v>0.3</v>
+      </c>
+      <c r="G30" t="s">
+        <v>54</v>
+      </c>
+      <c r="H30" t="s">
+        <v>53</v>
+      </c>
+      <c r="I30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" t="b">
+        <v>1</v>
+      </c>
+      <c r="L30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>0.9721378839636446</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31">
+        <v>123</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>172</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>0.1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>52</v>
+      </c>
+      <c r="H31" t="s">
+        <v>55</v>
+      </c>
+      <c r="I31" t="b">
+        <v>0</v>
+      </c>
+      <c r="J31" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31" t="b">
+        <v>0</v>
+      </c>
+      <c r="L31" t="b">
+        <v>1</v>
+      </c>
+      <c r="M31" t="b">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0.9705450966555303</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="B32">
+        <v>195</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>94</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>0.1</v>
+      </c>
+      <c r="G32" t="s">
+        <v>54</v>
+      </c>
+      <c r="H32" t="s">
+        <v>55</v>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" t="b">
+        <v>1</v>
+      </c>
+      <c r="L32" t="b">
+        <v>0</v>
+      </c>
+      <c r="M32" t="b">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0.9714854323864982</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="B33">
+        <v>68</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>230</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>0.2</v>
+      </c>
+      <c r="G33" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33" t="b">
+        <v>0</v>
+      </c>
+      <c r="J33" t="b">
+        <v>1</v>
+      </c>
+      <c r="K33" t="b">
+        <v>0</v>
+      </c>
+      <c r="L33" t="b">
+        <v>0</v>
+      </c>
+      <c r="M33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0.9901712807459832</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="B34">
+        <v>116</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>255</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <v>0.5</v>
+      </c>
+      <c r="G34" t="s">
+        <v>54</v>
+      </c>
+      <c r="H34" t="s">
+        <v>53</v>
+      </c>
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" t="b">
+        <v>0</v>
+      </c>
+      <c r="L34" t="b">
+        <v>0</v>
+      </c>
+      <c r="M34" t="b">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>0.9814623059029655</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="B35">
+        <v>59</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>182</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>0.4</v>
+      </c>
+      <c r="G35" t="s">
+        <v>54</v>
+      </c>
+      <c r="H35" t="s">
+        <v>53</v>
+      </c>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J35" t="b">
+        <v>0</v>
+      </c>
+      <c r="K35" t="b">
+        <v>0</v>
+      </c>
+      <c r="L35" t="b">
+        <v>0</v>
+      </c>
+      <c r="M35" t="b">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0.9509918688139359</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="B36">
+        <v>202</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>205</v>
+      </c>
+      <c r="E36">
+        <v>8</v>
+      </c>
+      <c r="F36">
+        <v>0.1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>54</v>
+      </c>
+      <c r="H36" t="s">
+        <v>56</v>
+      </c>
+      <c r="I36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J36" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" t="b">
+        <v>1</v>
+      </c>
+      <c r="L36" t="b">
+        <v>1</v>
+      </c>
+      <c r="M36" t="b">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <v>0.9454221195145931</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="B37">
+        <v>213</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>71</v>
+      </c>
+      <c r="E37">
+        <v>4</v>
+      </c>
+      <c r="F37">
+        <v>0.1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>54</v>
+      </c>
+      <c r="H37" t="s">
+        <v>55</v>
+      </c>
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" t="b">
+        <v>1</v>
+      </c>
+      <c r="K37" t="b">
+        <v>1</v>
+      </c>
+      <c r="L37" t="b">
+        <v>1</v>
+      </c>
+      <c r="M37" t="b">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>0.9341190211528081</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="B38">
+        <v>89</v>
+      </c>
+      <c r="C38">
+        <v>227</v>
+      </c>
+      <c r="D38">
+        <v>192</v>
+      </c>
+      <c r="E38">
+        <v>4</v>
+      </c>
+      <c r="F38">
+        <v>0.5</v>
+      </c>
+      <c r="G38" t="s">
+        <v>54</v>
+      </c>
+      <c r="H38" t="s">
+        <v>53</v>
+      </c>
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" t="b">
+        <v>1</v>
+      </c>
+      <c r="K38" t="b">
+        <v>0</v>
+      </c>
+      <c r="L38" t="b">
+        <v>1</v>
+      </c>
+      <c r="M38" t="b">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>0.9716147440814027</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="B39">
+        <v>59</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>65</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>0.2</v>
+      </c>
+      <c r="G39" t="s">
+        <v>52</v>
+      </c>
+      <c r="H39" t="s">
+        <v>53</v>
+      </c>
+      <c r="I39" t="b">
+        <v>0</v>
+      </c>
+      <c r="J39" t="b">
+        <v>1</v>
+      </c>
+      <c r="K39" t="b">
+        <v>0</v>
+      </c>
+      <c r="L39" t="b">
+        <v>0</v>
+      </c>
+      <c r="M39" t="b">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>0.8869172637649005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -754,14 +2251,14 @@
       <c r="E40">
         <v>4</v>
       </c>
-      <c r="F40" t="s">
-        <v>51</v>
+      <c r="F40">
+        <v>0.1</v>
       </c>
       <c r="G40" t="s">
         <v>52</v>
       </c>
-      <c r="H40" t="b">
-        <v>0</v>
+      <c r="H40" t="s">
+        <v>55</v>
       </c>
       <c r="I40" t="b">
         <v>0</v>
@@ -775,7 +2272,10 @@
       <c r="L40" t="b">
         <v>0</v>
       </c>
-      <c r="M40">
+      <c r="M40" t="b">
+        <v>0</v>
+      </c>
+      <c r="N40">
         <v>0.9570750098222738</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Dockerfile. Changed serialization to json
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -19,108 +19,108 @@
     <t>AAPL</t>
   </si>
   <si>
+    <t>MSFT</t>
+  </si>
+  <si>
+    <t>TSLA</t>
+  </si>
+  <si>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>KO</t>
+  </si>
+  <si>
+    <t>MCD</t>
+  </si>
+  <si>
+    <t>SBUX</t>
+  </si>
+  <si>
+    <t>AMZN</t>
+  </si>
+  <si>
     <t>ADBE</t>
   </si>
   <si>
+    <t>CMCSA</t>
+  </si>
+  <si>
+    <t>JNJ</t>
+  </si>
+  <si>
+    <t>DIS</t>
+  </si>
+  <si>
+    <t>INTC</t>
+  </si>
+  <si>
+    <t>NVDA</t>
+  </si>
+  <si>
     <t>AMD</t>
   </si>
   <si>
-    <t>AMZN</t>
+    <t>PFE</t>
+  </si>
+  <si>
+    <t>PEP</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>RACE</t>
+  </si>
+  <si>
+    <t>META</t>
+  </si>
+  <si>
+    <t>GOOG</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>GD</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>ORCL</t>
+  </si>
+  <si>
+    <t>PYPL</t>
+  </si>
+  <si>
+    <t>NKE</t>
   </si>
   <si>
     <t>AXP</t>
   </si>
   <si>
-    <t>BA</t>
-  </si>
-  <si>
     <t>BEN</t>
   </si>
   <si>
     <t>BKNG</t>
   </si>
   <si>
-    <t>CAT</t>
-  </si>
-  <si>
     <t>CL</t>
   </si>
   <si>
-    <t>CMCSA</t>
-  </si>
-  <si>
     <t>DAL</t>
   </si>
   <si>
-    <t>DIS</t>
-  </si>
-  <si>
     <t>DPZ</t>
   </si>
   <si>
     <t>EA</t>
   </si>
   <si>
-    <t>GD</t>
-  </si>
-  <si>
-    <t>GE</t>
-  </si>
-  <si>
-    <t>GM</t>
-  </si>
-  <si>
-    <t>GOOG</t>
-  </si>
-  <si>
-    <t>INTC</t>
-  </si>
-  <si>
-    <t>JNJ</t>
-  </si>
-  <si>
-    <t>KO</t>
-  </si>
-  <si>
-    <t>MA</t>
-  </si>
-  <si>
-    <t>MCD</t>
-  </si>
-  <si>
-    <t>META</t>
-  </si>
-  <si>
-    <t>MSFT</t>
-  </si>
-  <si>
-    <t>NKE</t>
-  </si>
-  <si>
-    <t>NVDA</t>
-  </si>
-  <si>
-    <t>ORCL</t>
-  </si>
-  <si>
-    <t>PEP</t>
-  </si>
-  <si>
-    <t>PFE</t>
-  </si>
-  <si>
-    <t>PYPL</t>
-  </si>
-  <si>
-    <t>RACE</t>
-  </si>
-  <si>
-    <t>SBUX</t>
-  </si>
-  <si>
-    <t>TSLA</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
@@ -178,10 +178,10 @@
     <t>adam</t>
   </si>
   <si>
+    <t>adamax</t>
+  </si>
+  <si>
     <t>mse</t>
-  </si>
-  <si>
-    <t>adamax</t>
   </si>
   <si>
     <t>rmsprop</t>
@@ -612,43 +612,43 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>134</v>
+        <v>203</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F3">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="G3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" t="s">
         <v>54</v>
       </c>
-      <c r="H3" t="s">
-        <v>55</v>
-      </c>
       <c r="I3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" t="b">
         <v>1</v>
       </c>
       <c r="M3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3">
-        <v>0.9501156745476711</v>
+        <v>0.9806609146551855</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -656,43 +656,43 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>338</v>
+        <v>202</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F4">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="b">
         <v>0</v>
       </c>
       <c r="K4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" t="b">
         <v>1</v>
       </c>
       <c r="M4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>0.9582699610737877</v>
+        <v>0.9454221195145931</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -700,28 +700,28 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="C5">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>125</v>
+        <v>235</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="G5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" t="s">
         <v>54</v>
       </c>
-      <c r="H5" t="s">
-        <v>53</v>
-      </c>
       <c r="I5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="b">
         <v>0</v>
@@ -730,13 +730,13 @@
         <v>0</v>
       </c>
       <c r="L5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" t="b">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.9504124330538782</v>
+        <v>0.971156190647037</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -744,43 +744,43 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>246</v>
+        <v>135</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6" t="b">
         <v>1</v>
       </c>
       <c r="M6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>0.96115939006122</v>
+        <v>0.954180614849984</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -788,22 +788,22 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>146</v>
+        <v>289</v>
       </c>
       <c r="C7">
-        <v>158</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H7" t="s">
         <v>53</v>
@@ -812,19 +812,19 @@
         <v>1</v>
       </c>
       <c r="J7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" t="b">
         <v>0</v>
       </c>
       <c r="M7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>0.9081919883983061</v>
+        <v>0.9751283418089106</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -832,43 +832,43 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>86</v>
+        <v>182</v>
       </c>
       <c r="E8">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H8" t="s">
         <v>53</v>
       </c>
       <c r="I8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" t="b">
         <v>0</v>
       </c>
       <c r="M8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>0.9267131303970635</v>
+        <v>0.9509918688139359</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -876,22 +876,22 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>249</v>
+        <v>160</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="D9">
-        <v>200</v>
+        <v>125</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
         <v>53</v>
@@ -906,13 +906,13 @@
         <v>0</v>
       </c>
       <c r="L9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>0.9672992986824098</v>
+        <v>0.9504124330538782</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -920,28 +920,28 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>235</v>
+        <v>134</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="G10" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="b">
         <v>0</v>
@@ -956,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0.971156190647037</v>
+        <v>0.9501156745476711</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -964,22 +964,22 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>169</v>
+        <v>257</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="E11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H11" t="s">
         <v>53</v>
@@ -994,13 +994,13 @@
         <v>0</v>
       </c>
       <c r="L11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" t="b">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0.8755700150909251</v>
+        <v>0.968225173952287</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1008,22 +1008,22 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>257</v>
+        <v>81</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>123</v>
+        <v>228</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F12">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="G12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H12" t="s">
         <v>53</v>
@@ -1044,7 +1044,7 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>0.968225173952287</v>
+        <v>0.9117900192688089</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1052,43 +1052,43 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>153</v>
+        <v>205</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F13">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="G13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" t="s">
         <v>54</v>
       </c>
-      <c r="H13" t="s">
-        <v>53</v>
-      </c>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13">
-        <v>0.8966909817822324</v>
+        <v>0.9799557670400426</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1096,43 +1096,43 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>205</v>
+        <v>91</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="E14">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G14" t="s">
         <v>52</v>
       </c>
       <c r="H14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" t="b">
         <v>0</v>
       </c>
       <c r="L14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14">
-        <v>0.9799557670400426</v>
+        <v>0.9688477999079659</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -1140,25 +1140,25 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>52</v>
+        <v>217</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>219</v>
+        <v>61</v>
       </c>
       <c r="E15">
         <v>3</v>
       </c>
       <c r="F15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G15" t="s">
         <v>52</v>
       </c>
       <c r="H15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
@@ -1170,13 +1170,13 @@
         <v>0</v>
       </c>
       <c r="L15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" t="b">
         <v>0</v>
       </c>
       <c r="N15">
-        <v>0.9544293863133937</v>
+        <v>0.9899385797607924</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -1184,43 +1184,43 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>110</v>
+        <v>338</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>90</v>
+        <v>202</v>
       </c>
       <c r="E16">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F16">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="G16" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
       </c>
       <c r="J16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" t="b">
         <v>1</v>
       </c>
       <c r="M16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16">
-        <v>0.8251011798612152</v>
+        <v>0.9582699610737877</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -1228,34 +1228,34 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>86</v>
+        <v>195</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>149</v>
+        <v>94</v>
       </c>
       <c r="E17">
         <v>3</v>
       </c>
       <c r="F17">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="G17" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" t="b">
         <v>0</v>
@@ -1264,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="N17">
-        <v>0.9822583871954536</v>
+        <v>0.9714854323864982</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1272,31 +1272,31 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>254</v>
+        <v>123</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>131</v>
+        <v>172</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F18">
         <v>0.1</v>
       </c>
       <c r="G18" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" t="s">
         <v>54</v>
       </c>
-      <c r="H18" t="s">
-        <v>53</v>
-      </c>
       <c r="I18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" t="b">
         <v>0</v>
@@ -1308,7 +1308,7 @@
         <v>0</v>
       </c>
       <c r="N18">
-        <v>0.9901075522078303</v>
+        <v>0.9705450966555303</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1334,7 +1334,7 @@
         <v>52</v>
       </c>
       <c r="H19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I19" t="b">
         <v>0</v>
@@ -1360,22 +1360,22 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>233</v>
+        <v>146</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>158</v>
       </c>
       <c r="D20">
-        <v>245</v>
+        <v>150</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="G20" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H20" t="s">
         <v>53</v>
@@ -1396,7 +1396,7 @@
         <v>1</v>
       </c>
       <c r="N20">
-        <v>0.9709357499660785</v>
+        <v>0.9081919883983061</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1404,28 +1404,28 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
-        <v>108</v>
+        <v>255</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F21">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G21" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="b">
         <v>0</v>
@@ -1437,10 +1437,10 @@
         <v>0</v>
       </c>
       <c r="M21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21">
-        <v>0.9688477999079659</v>
+        <v>0.9814623059029655</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1448,22 +1448,22 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>81</v>
+        <v>222</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>228</v>
+        <v>75</v>
       </c>
       <c r="E22">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="G22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H22" t="s">
         <v>53</v>
@@ -1484,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="N22">
-        <v>0.9117900192688089</v>
+        <v>0.9813957773311417</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -1492,43 +1492,43 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>70</v>
+        <v>233</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>135</v>
+        <v>245</v>
       </c>
       <c r="E23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H23" t="s">
         <v>53</v>
       </c>
       <c r="I23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23">
-        <v>0.954180614849984</v>
+        <v>0.9709357499660785</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1536,31 +1536,31 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>211</v>
+        <v>254</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="E24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F24">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G24" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H24" t="s">
         <v>53</v>
       </c>
       <c r="I24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" t="b">
         <v>0</v>
@@ -1572,7 +1572,7 @@
         <v>0</v>
       </c>
       <c r="N24">
-        <v>0.9239992251801622</v>
+        <v>0.9901075522078303</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -1580,31 +1580,31 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>289</v>
+        <v>86</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E25">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F25">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="G25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H25" t="s">
         <v>53</v>
       </c>
       <c r="I25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" t="b">
         <v>0</v>
@@ -1616,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="N25">
-        <v>0.9751283418089106</v>
+        <v>0.9822583871954536</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1624,22 +1624,22 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E26">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F26">
         <v>0.5</v>
       </c>
       <c r="G26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H26" t="s">
         <v>53</v>
@@ -1654,13 +1654,13 @@
         <v>0</v>
       </c>
       <c r="L26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26" t="b">
         <v>0</v>
       </c>
       <c r="N26">
-        <v>0.9813957773311417</v>
+        <v>0.9239992251801622</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -1668,28 +1668,28 @@
         <v>25</v>
       </c>
       <c r="B27">
+        <v>139</v>
+      </c>
+      <c r="C27">
+        <v>69</v>
+      </c>
+      <c r="D27">
+        <v>111</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>0.3</v>
+      </c>
+      <c r="G27" t="s">
         <v>55</v>
       </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>203</v>
-      </c>
-      <c r="E27">
-        <v>10</v>
-      </c>
-      <c r="F27">
-        <v>0.4</v>
-      </c>
-      <c r="G27" t="s">
-        <v>52</v>
-      </c>
       <c r="H27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="b">
         <v>1</v>
@@ -1698,13 +1698,13 @@
         <v>1</v>
       </c>
       <c r="L27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N27">
-        <v>0.9806609146551855</v>
+        <v>0.9721378839636446</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -1712,43 +1712,43 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>117</v>
+        <v>68</v>
       </c>
       <c r="C28">
-        <v>233</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="E28">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F28">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G28" t="s">
         <v>52</v>
       </c>
       <c r="H28" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="b">
         <v>1</v>
       </c>
       <c r="K28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N28">
-        <v>0.9576394501923923</v>
+        <v>0.9901712807459832</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -1756,19 +1756,19 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>217</v>
+        <v>117</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>233</v>
       </c>
       <c r="D29">
-        <v>61</v>
+        <v>212</v>
       </c>
       <c r="E29">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F29">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G29" t="s">
         <v>52</v>
@@ -1777,22 +1777,22 @@
         <v>53</v>
       </c>
       <c r="I29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L29" t="b">
         <v>1</v>
       </c>
       <c r="M29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N29">
-        <v>0.9899385797607924</v>
+        <v>0.9576394501923923</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -1800,28 +1800,28 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>139</v>
+        <v>93</v>
       </c>
       <c r="C30">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>111</v>
+        <v>246</v>
       </c>
       <c r="E30">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F30">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="G30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H30" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" t="b">
         <v>1</v>
@@ -1830,13 +1830,13 @@
         <v>1</v>
       </c>
       <c r="L30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N30">
-        <v>0.9721378839636446</v>
+        <v>0.96115939006122</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -1844,43 +1844,43 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>123</v>
+        <v>67</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31">
-        <v>172</v>
+        <v>86</v>
       </c>
       <c r="E31">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F31">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G31" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I31" t="b">
         <v>0</v>
       </c>
       <c r="J31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N31">
-        <v>0.9705450966555303</v>
+        <v>0.9267131303970635</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -1888,43 +1888,43 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>195</v>
+        <v>249</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>94</v>
+        <v>200</v>
       </c>
       <c r="E32">
         <v>3</v>
       </c>
       <c r="F32">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="G32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="b">
         <v>0</v>
       </c>
       <c r="K32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N32">
-        <v>0.9714854323864982</v>
+        <v>0.9672992986824098</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -1932,43 +1932,43 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>68</v>
+        <v>169</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33">
-        <v>230</v>
+        <v>114</v>
       </c>
       <c r="E33">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F33">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G33" t="s">
         <v>52</v>
       </c>
       <c r="H33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I33" t="b">
         <v>0</v>
       </c>
       <c r="J33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33" t="b">
         <v>0</v>
       </c>
       <c r="L33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" t="b">
         <v>0</v>
       </c>
       <c r="N33">
-        <v>0.9901712807459832</v>
+        <v>0.8755700150909251</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -1976,43 +1976,43 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>255</v>
+        <v>132</v>
       </c>
       <c r="E34">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F34">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G34" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H34" t="s">
         <v>53</v>
       </c>
       <c r="I34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="b">
         <v>0</v>
       </c>
       <c r="K34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L34" t="b">
         <v>0</v>
       </c>
       <c r="M34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N34">
-        <v>0.9814623059029655</v>
+        <v>0.8966909817822324</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -2020,28 +2020,28 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>182</v>
+        <v>219</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F35">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="G35" t="s">
+        <v>52</v>
+      </c>
+      <c r="H35" t="s">
         <v>54</v>
       </c>
-      <c r="H35" t="s">
-        <v>53</v>
-      </c>
       <c r="I35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" t="b">
         <v>0</v>
@@ -2056,7 +2056,7 @@
         <v>0</v>
       </c>
       <c r="N35">
-        <v>0.9509918688139359</v>
+        <v>0.9544293863133937</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -2064,31 +2064,31 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>202</v>
+        <v>110</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>205</v>
+        <v>90</v>
       </c>
       <c r="E36">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F36">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="G36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H36" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" t="b">
         <v>1</v>
@@ -2100,7 +2100,7 @@
         <v>1</v>
       </c>
       <c r="N36">
-        <v>0.9454221195145931</v>
+        <v>0.8251011798612152</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -2123,10 +2123,10 @@
         <v>0.1</v>
       </c>
       <c r="G37" t="s">
+        <v>55</v>
+      </c>
+      <c r="H37" t="s">
         <v>54</v>
-      </c>
-      <c r="H37" t="s">
-        <v>55</v>
       </c>
       <c r="I37" t="b">
         <v>1</v>
@@ -2167,7 +2167,7 @@
         <v>0.5</v>
       </c>
       <c r="G38" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H38" t="s">
         <v>53</v>
@@ -2258,7 +2258,7 @@
         <v>52</v>
       </c>
       <c r="H40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I40" t="b">
         <v>0</v>

</xml_diff>